<commit_message>
Implemented accuracy checking. Accuracy is terrible and low
</commit_message>
<xml_diff>
--- a/monitor_data.xlsx
+++ b/monitor_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\University courses\University 2024 Tri1\ENGR489\ocr-for-anaesthesia-monitors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9893C79D-9652-4109-B9A0-9156C75D0C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79807E48-A8A9-4DCA-896E-0B7A654F2095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0333338E-0FE0-4831-82AE-614B044C1483}"/>
   </bookViews>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03441698-D578-4B5E-B47F-A718E32EBBD5}">
   <dimension ref="A1:J183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="N178" sqref="N178"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="C186" sqref="C186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>